<commit_message>
Add rrdfancillary a lot of places... - builds
</commit_message>
<xml_diff>
--- a/rrdfqbcrndex/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
+++ b/rrdfqbcrndex/inst/extdata/sample-cfg/RDFCubeWorkbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DEMO-Components" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,11 +16,16 @@
     <sheet name="CubePrefixes" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="145">
   <si>
     <t>compType</t>
   </si>
@@ -450,6 +455,12 @@
   </si>
   <si>
     <t>http://www.example.org/rrdfqbcrnd0/</t>
+  </si>
+  <si>
+    <t>sdtm</t>
+  </si>
+  <si>
+    <t>http://rdf.cdisc.org/sdtm-terminology#</t>
   </si>
 </sst>
 </file>
@@ -816,18 +827,18 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A11:E13"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.70918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="81.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="80.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,15 +1291,15 @@
   <dimension ref="1:13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A11:E13"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="83.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="6" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="82.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="6" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,16 +3440,16 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A11:E13 A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="65.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="55.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="6" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="64.7959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="55.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="6" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3833,17 +3844,17 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11:E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="65.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="41"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="6" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="64.7959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="40.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="6" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4281,16 +4292,16 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="1" sqref="A11:E13 B41"/>
+      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="18.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="23.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="26.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="6" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="6" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="6" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4537,17 +4548,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A11:E13 B19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="43.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="6" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="42.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="6" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4668,6 +4679,14 @@
       </c>
       <c r="B15" s="22" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>